<commit_message>
adds test for previously geocoded functionality
</commit_message>
<xml_diff>
--- a/excel_files/housing_addendum.xlsx
+++ b/excel_files/housing_addendum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for_db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0D3C8A-78A6-484F-B883-585647A4A860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68CF42A-4677-374C-8B2D-B8CF5100B33B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H-2A_ADDEN_B_HOUSING_FY2020Q3" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>CASE_NUMBER</t>
   </si>
@@ -101,12 +101,6 @@
     <t>UTAH</t>
   </si>
   <si>
-    <t>250 South 300 West</t>
-  </si>
-  <si>
-    <t>Santaquin</t>
-  </si>
-  <si>
     <t>H-300-19291-095211</t>
   </si>
   <si>
@@ -114,15 +108,6 @@
   </si>
   <si>
     <t>Conventional frame house</t>
-  </si>
-  <si>
-    <t>212 1st Street</t>
-  </si>
-  <si>
-    <t>Towner</t>
-  </si>
-  <si>
-    <t>NORTH DAKOTA</t>
   </si>
   <si>
     <t>MCHENRY</t>
@@ -271,6 +256,27 @@
   <si>
     <t>HOUSING_COUNTY</t>
   </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>Lanechester</t>
+  </si>
+  <si>
+    <t>1 Alstede Farms</t>
+  </si>
+  <si>
+    <t>new jersey</t>
+  </si>
+  <si>
+    <t>New jersey</t>
+  </si>
+  <si>
+    <t>farmingdale</t>
+  </si>
+  <si>
+    <t>101 Havens bridge RD</t>
+  </si>
 </sst>
 </file>
 
@@ -412,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +598,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -753,11 +765,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1081,9 +1094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O12901"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1116,25 +1129,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" t="s">
-        <v>78</v>
-      </c>
       <c r="J1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K1" t="s">
         <v>3</v>
@@ -1143,13 +1156,13 @@
         <v>4</v>
       </c>
       <c r="M1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="O1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1237,115 +1250,115 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7930</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>15</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
-        <v>21</v>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
       </c>
-      <c r="H4">
-        <v>84655</v>
+      <c r="D5" s="2" t="s">
+        <v>80</v>
       </c>
-      <c r="I4" t="s">
-        <v>21</v>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
       </c>
-      <c r="K4">
+      <c r="G5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="2">
+        <v>7727</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>15</v>
+      <c r="L5" s="2">
+        <v>3</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
         <v>27</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="H5">
-        <v>58788</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="G6" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
       </c>
       <c r="H6">
         <v>72342</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1365,31 +1378,31 @@
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>96101</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -1409,31 +1422,31 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8">
         <v>81647</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1453,31 +1466,31 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H9">
         <v>83254</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K9">
         <v>6</v>
@@ -1497,28 +1510,28 @@
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="H10">
         <v>80651</v>
       </c>
       <c r="I10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1538,28 +1551,28 @@
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H11">
         <v>80621</v>
       </c>
       <c r="I11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K11">
         <v>1</v>

</xml_diff>